<commit_message>
test for cost/schedule matrix. passing. matplotlib scatter charted first commit
</commit_message>
<xml_diff>
--- a/tests/resources/test_dandelion_data.xlsx
+++ b/tests/resources/test_dandelion_data.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,20 +356,15 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Group</t>
+          <t>Project details</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Project</t>
+          <t>WLC (forecast)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
-        <is>
-          <t>WLC (forecast)</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
         <is>
           <t>DCA</t>
         </is>
@@ -378,18 +373,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Roads Devolution &amp; Motoring</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SoT, £3,1bn</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3067</v>
-      </c>
-      <c r="D2" t="inlineStr">
+          <t>A11,
+£90m</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>89</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -398,18 +389,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rail Group</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A11, £90m</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>89</v>
-      </c>
-      <c r="D3" t="inlineStr">
+          <t>Columbia,
+£4,3bn</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4345</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -418,58 +405,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rail Group</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A13, £89,8bn</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+          <t>A13,
+£89,8bn</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>89809</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Roads Devolution &amp; Motoring</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>F9, £87,9bn</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>87879</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rail Group</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Columbia, £4,3bn</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4345</v>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Green</t>
         </is>

</xml_diff>